<commit_message>
ER-Modell changed and updated
</commit_message>
<xml_diff>
--- a/documentation/ER-Modell Tabellen.xlsx
+++ b/documentation/ER-Modell Tabellen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Desktop\Diplomarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Desktop\Diplomarbeit2\game\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E067AD9-001F-4CB0-899D-58D24693EFA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4DF799-FB15-426C-BF81-89E1B016701C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E9E2E99E-C2C0-475F-924D-D96A81B2B5AB}"/>
+    <workbookView xWindow="-5232" yWindow="4416" windowWidth="10488" windowHeight="9960" xr2:uid="{E9E2E99E-C2C0-475F-924D-D96A81B2B5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -297,23 +297,23 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -631,7 +631,7 @@
   <dimension ref="A2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,470 +650,470 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="3">
-        <v>1</v>
-      </c>
-      <c r="K12" s="3" t="s">
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>4</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="3">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="3">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="F18" s="3" t="s">
+      <c r="A18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="F18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="2">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="3">
-        <v>2</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F22" s="3">
-        <v>2</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="F23" s="3">
+      <c r="B23" s="6"/>
+      <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>3</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>2</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
-        <v>1</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="A32" s="2">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2">
         <v>3</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3">
+      <c r="A34" s="2">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2">
         <v>4</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
-        <v>2</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="A35" s="2">
+        <v>2</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
-        <v>2</v>
-      </c>
-      <c r="B36" s="3">
-        <v>2</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="A36" s="2">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
-        <v>2</v>
-      </c>
-      <c r="B37" s="3">
+      <c r="A37" s="2">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2">
         <v>3</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
-        <v>2</v>
-      </c>
-      <c r="B38" s="3">
+      <c r="A38" s="2">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2">
         <v>4</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="F10:K10"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>